<commit_message>
Added long pins header
</commit_message>
<xml_diff>
--- a/PCBV4.1/OxFloodNet_Sensor_BOM.xlsx
+++ b/PCBV4.1/OxFloodNet_Sensor_BOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="83">
   <si>
     <t>Oxford Flood Network Sensor: Bill of materials</t>
   </si>
@@ -98,7 +98,13 @@
     <t>HDR1</t>
   </si>
   <si>
-    <t>1x7W Header</t>
+    <t>1x7W Header - Long Pins (8W stackable header)</t>
+  </si>
+  <si>
+    <t>Bitsbox</t>
+  </si>
+  <si>
+    <t>CN312</t>
   </si>
   <si>
     <t>MAXBOTIX-MB1</t>
@@ -216,6 +222,9 @@
   </si>
   <si>
     <t>Antenna wire, 90mm (Gauge???)</t>
+  </si>
+  <si>
+    <t>Already have some of this from last time</t>
   </si>
   <si>
     <t>ANT2</t>
@@ -234,7 +243,7 @@
       <rPr>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>uk.farnell.com</t>
@@ -245,7 +254,7 @@
       <rPr>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>shop.ciseco.co.uk</t>
@@ -256,7 +265,7 @@
       <rPr>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>thinginnovations.com</t>
@@ -273,7 +282,7 @@
       <rPr>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>www.technobotsonline.com</t>
@@ -284,10 +293,21 @@
       <rPr>
         <u val="single"/>
         <sz val="11"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Calibri"/>
       </rPr>
       <t>www.batterystation.co.uk</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="11"/>
+        <color indexed="14"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>www.bitsbox.co.uk</t>
     </r>
   </si>
 </sst>
@@ -298,7 +318,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -343,6 +363,11 @@
       <name val="Courier New,courier"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <u val="single"/>
       <sz val="11"/>
@@ -357,13 +382,19 @@
     </font>
     <font>
       <sz val="11"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="11"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color indexed="14"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -647,7 +678,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -717,31 +748,34 @@
     <xf numFmtId="0" fontId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="8" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="2" fontId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="9" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="3" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="9" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
     <xf numFmtId="0" fontId="10" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -764,7 +798,9 @@
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ff111111"/>
       <rgbColor rgb="ff4f81bd"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -2256,17 +2292,16 @@
         <v>1</v>
       </c>
       <c r="D11" t="s" s="18">
-        <v>16</v>
-      </c>
-      <c r="E11" s="19">
-        <v>2308805</v>
+        <v>29</v>
+      </c>
+      <c r="E11" t="s" s="23">
+        <v>30</v>
       </c>
       <c r="F11" s="20">
-        <v>0.54</v>
+        <v>0.4</v>
       </c>
       <c r="G11" s="20">
-        <f>C11*F11</f>
-        <v>0.54</v>
+        <v>0.4</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="3"/>
@@ -2274,10 +2309,10 @@
     </row>
     <row r="12" ht="17" customHeight="1">
       <c r="A12" t="s" s="17">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s" s="18">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C12" s="18">
         <v>1</v>
@@ -2286,7 +2321,7 @@
         <v>16</v>
       </c>
       <c r="E12" t="s" s="19">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F12" s="20">
         <v>1.29</v>
@@ -2296,17 +2331,17 @@
         <v>1.29</v>
       </c>
       <c r="H12" t="s" s="20">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
     <row r="13" ht="17" customHeight="1">
       <c r="A13" t="s" s="17">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s" s="18">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" s="18">
         <v>1</v>
@@ -2330,10 +2365,10 @@
     </row>
     <row r="14" ht="17" customHeight="1">
       <c r="A14" t="s" s="17">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s" s="18">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" s="18">
         <v>1</v>
@@ -2357,10 +2392,10 @@
     </row>
     <row r="15" ht="17" customHeight="1">
       <c r="A15" t="s" s="17">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s" s="18">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" s="18">
         <v>2</v>
@@ -2384,10 +2419,10 @@
     </row>
     <row r="16" ht="17" customHeight="1">
       <c r="A16" t="s" s="17">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s" s="18">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" s="18">
         <v>1</v>
@@ -2411,19 +2446,19 @@
     </row>
     <row r="17" ht="17" customHeight="1">
       <c r="A17" t="s" s="17">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s" s="18">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C17" s="18">
         <v>1</v>
       </c>
       <c r="D17" t="s" s="18">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s" s="19">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F17" s="20">
         <v>13.99</v>
@@ -2438,19 +2473,19 @@
     </row>
     <row r="18" ht="17" customHeight="1">
       <c r="A18" t="s" s="17">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B18" t="s" s="18">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C18" s="18">
         <v>1</v>
       </c>
       <c r="D18" t="s" s="18">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E18" t="s" s="19">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F18" s="20">
         <v>76.16</v>
@@ -2465,19 +2500,19 @@
     </row>
     <row r="19" ht="17" customHeight="1">
       <c r="A19" t="s" s="17">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s" s="18">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C19" s="18">
         <v>1</v>
       </c>
       <c r="D19" t="s" s="18">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E19" t="s" s="19">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F19" s="20">
         <v>1.88</v>
@@ -2492,19 +2527,19 @@
     </row>
     <row r="20" ht="17" customHeight="1">
       <c r="A20" t="s" s="17">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s" s="18">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C20" s="18">
         <v>1</v>
       </c>
       <c r="D20" t="s" s="18">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s" s="19">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F20" s="20">
         <v>2.55</v>
@@ -2519,19 +2554,19 @@
     </row>
     <row r="21" ht="17" customHeight="1">
       <c r="A21" t="s" s="17">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B21" t="s" s="18">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C21" s="18">
         <v>0.5</v>
       </c>
       <c r="D21" t="s" s="18">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="E21" t="s" s="19">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F21" s="20">
         <v>1.06</v>
@@ -2546,10 +2581,10 @@
     </row>
     <row r="22" ht="17" customHeight="1">
       <c r="A22" t="s" s="17">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B22" t="s" s="18">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C22" s="18">
         <v>2</v>
@@ -2558,7 +2593,7 @@
         <v>16</v>
       </c>
       <c r="E22" t="s" s="19">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F22" s="20">
         <v>0.22</v>
@@ -2573,19 +2608,19 @@
     </row>
     <row r="23" ht="17" customHeight="1">
       <c r="A23" t="s" s="17">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s" s="18">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C23" s="18">
         <v>1</v>
       </c>
       <c r="D23" t="s" s="18">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="E23" t="s" s="19">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="20">
@@ -2598,10 +2633,10 @@
     </row>
     <row r="24" ht="17" customHeight="1">
       <c r="A24" t="s" s="17">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B24" t="s" s="18">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C24" s="18">
         <v>1</v>
@@ -2609,30 +2644,32 @@
       <c r="D24" t="s" s="18">
         <v>16</v>
       </c>
-      <c r="E24" s="23"/>
+      <c r="E24" s="24"/>
       <c r="F24" s="3"/>
       <c r="G24" s="20">
         <f>C24*F24</f>
         <v>0</v>
       </c>
-      <c r="H24" s="3"/>
+      <c r="H24" t="s" s="20">
+        <v>70</v>
+      </c>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
     <row r="25" ht="17" customHeight="1">
       <c r="A25" t="s" s="17">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s" s="18">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="C25" s="18">
         <v>1</v>
       </c>
       <c r="D25" t="s" s="18">
-        <v>70</v>
-      </c>
-      <c r="E25" s="23"/>
+        <v>73</v>
+      </c>
+      <c r="E25" s="24"/>
       <c r="F25" s="3"/>
       <c r="G25" s="20">
         <f>C25*F25</f>
@@ -2643,26 +2680,26 @@
       <c r="J25" s="3"/>
     </row>
     <row r="26" ht="17" customHeight="1">
-      <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14">
         <f>SUM(G5:G25)</f>
-        <v>108.49</v>
+        <v>108.35</v>
       </c>
       <c r="H26" s="20"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
     <row r="27" ht="15" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="28"/>
+      <c r="A27" s="27"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
       <c r="H27" s="20"/>
@@ -2686,17 +2723,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.625" defaultRowHeight="14.4" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="14.75" style="29" customWidth="1"/>
-    <col min="2" max="2" width="20.625" style="29" customWidth="1"/>
-    <col min="3" max="3" width="17.75" style="29" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="29" customWidth="1"/>
-    <col min="5" max="5" width="6.625" style="29" customWidth="1"/>
-    <col min="6" max="256" width="6.625" style="29" customWidth="1"/>
+    <col min="1" max="1" width="14.75" style="30" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="30" customWidth="1"/>
+    <col min="3" max="3" width="17.75" style="30" customWidth="1"/>
+    <col min="4" max="4" width="6.625" style="30" customWidth="1"/>
+    <col min="5" max="5" width="6.625" style="30" customWidth="1"/>
+    <col min="6" max="256" width="6.625" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="17" customHeight="1">
-      <c r="A1" t="s" s="30">
-        <v>71</v>
+      <c r="A1" t="s" s="31">
+        <v>74</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2707,8 +2744,8 @@
       <c r="A2" t="s" s="20">
         <v>16</v>
       </c>
-      <c r="B2" t="s" s="31">
-        <v>72</v>
+      <c r="B2" t="s" s="32">
+        <v>75</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2716,10 +2753,10 @@
     </row>
     <row r="3" ht="17" customHeight="1">
       <c r="A3" t="s" s="20">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s" s="31">
-        <v>73</v>
+        <v>45</v>
+      </c>
+      <c r="B3" t="s" s="32">
+        <v>76</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2729,21 +2766,21 @@
       <c r="A4" t="s" s="20">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="31">
-        <v>74</v>
+      <c r="B4" t="s" s="32">
+        <v>77</v>
       </c>
       <c r="C4" t="s" s="20">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" t="s" s="20">
-        <v>76</v>
-      </c>
-      <c r="B5" t="s" s="31">
-        <v>77</v>
+        <v>79</v>
+      </c>
+      <c r="B5" t="s" s="32">
+        <v>80</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -2751,18 +2788,22 @@
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" t="s" s="20">
-        <v>64</v>
-      </c>
-      <c r="B6" t="s" s="31">
-        <v>78</v>
+        <v>66</v>
+      </c>
+      <c r="B6" t="s" s="32">
+        <v>81</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
     <row r="7" ht="17" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+      <c r="A7" t="s" s="20">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s" s="20">
+        <v>82</v>
+      </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -2780,6 +2821,7 @@
     <hyperlink ref="B4" r:id="rId2" location="" tooltip="" display=""/>
     <hyperlink ref="B5" r:id="rId3" location="" tooltip="" display=""/>
     <hyperlink ref="B6" r:id="rId4" location="" tooltip="" display=""/>
+    <hyperlink ref="B7" r:id="rId5" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>